<commit_message>
Improved Optimize by starting at a no outage point.  Reduced iterations.
</commit_message>
<xml_diff>
--- a/Analysis/Iteration_count.xlsx
+++ b/Analysis/Iteration_count.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cd0e7a053322a97/Documents/GenAtomic/Optimize/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F922554-C1DB-4E57-BFEE-7A8329BC08CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{6F922554-C1DB-4E57-BFEE-7A8329BC08CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C63F6B29-535B-4801-BAA0-7C154FDAC6B2}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{0203C60F-354D-4E6D-A81C-B45BCF0A78B5}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Years</t>
-  </si>
-  <si>
     <t>Days</t>
   </si>
   <si>
@@ -50,13 +47,16 @@
     <t>regions</t>
   </si>
   <si>
-    <t>Out Year</t>
-  </si>
-  <si>
     <t>CO2</t>
   </si>
   <si>
     <t>Opt Runs</t>
+  </si>
+  <si>
+    <t>Output Years</t>
+  </si>
+  <si>
+    <t>Sample Years</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
   <cols>
-    <col min="1" max="1" width="5.03515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.34375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.65234375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.15234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.15234375" bestFit="1" customWidth="1"/>
@@ -449,25 +449,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.85">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.85">
@@ -487,10 +487,10 @@
         <v>26</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2">
-        <v>1500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.85">
@@ -512,11 +512,11 @@
       </c>
       <c r="F3" s="1">
         <f>PRODUCT($A$2:F2)</f>
-        <v>148145400</v>
+        <v>133330860</v>
       </c>
       <c r="G3" s="1">
         <f>PRODUCT($A$2:G2)</f>
-        <v>222218100000</v>
+        <v>93331602000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>